<commit_message>
new sheet desc to measures
</commit_message>
<xml_diff>
--- a/reports/corpus.xlsx
+++ b/reports/corpus.xlsx
@@ -5,16 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avitsas\Documents\playground\playground-new\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avitsas\Documents\thesis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50642DDD-EF38-4464-AE1E-C66ED6BC53CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B925FF-E899-49AD-9980-78789CB6B40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31950" yWindow="3435" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{187E2C83-AA30-4404-8C1D-88DFE9242203}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{187E2C83-AA30-4404-8C1D-88DFE9242203}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="corpus" sheetId="1" r:id="rId1"/>
     <sheet name="descriptions_measures" sheetId="2" r:id="rId2"/>
+    <sheet name="R1" sheetId="4" r:id="rId3"/>
+    <sheet name="R2" sheetId="5" r:id="rId4"/>
+    <sheet name="R3" sheetId="6" r:id="rId5"/>
+    <sheet name="R4" sheetId="7" r:id="rId6"/>
+    <sheet name="R5" sheetId="8" r:id="rId7"/>
+    <sheet name="R6" sheetId="3" r:id="rId8"/>
+    <sheet name="R7" sheetId="9" r:id="rId9"/>
+    <sheet name="R8" sheetId="10" r:id="rId10"/>
+    <sheet name="R9" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="93">
   <si>
     <t>Descriptions</t>
   </si>
@@ -253,6 +262,72 @@
   </si>
   <si>
     <t>Observation point number (customer)</t>
+  </si>
+  <si>
+    <t>MEAS_ACCH_AMT_PAYMENT_CP</t>
+  </si>
+  <si>
+    <t>MEAS_ACCL_SETTLEMENT_PAYMENT_PREDICTION_PAYERS_AMT</t>
+  </si>
+  <si>
+    <t>MEAS_ACCL_STRAY_PAYMENT_PREDICTION_PAYERS_AMT</t>
+  </si>
+  <si>
+    <t>MEAS_APPL_AMT_APPROVED</t>
+  </si>
+  <si>
+    <t>MEAS_APPL_AMT_PAYMENTS_TOTAL</t>
+  </si>
+  <si>
+    <t>MEAS_APPL_AMT_DISCOUNT</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_AMT_INSTALMENTS_FUTURE</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DURATION_UP_TO_6M</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DURATION_07_TO_12M</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DURATION_13_TO_36M</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DURATION_37_TO_72M</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DURATION_73_TO_108M</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DURATION_109_PLUS</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_AMT_ENTRY_PRINCIPAL</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_AMT_ENTRY_BALANCE</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>MEAS_APPL_AMT_WRITEOFF</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DAYS_APPROVED</t>
+  </si>
+  <si>
+    <t>MEAS_APPL_DURATION_APPROVED</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>MEAS_APLL_DAYS_REJECTED</t>
   </si>
 </sst>
 </file>
@@ -276,15 +351,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -292,11 +373,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -305,6 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,13 +1095,167 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99294B7E-0804-4329-AB8D-4885E2EC85E2}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94D4A56-ED64-4A15-A3F6-A8011B4A799E}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C4968E-0E08-41CF-89E0-C5CBE6AF71CA}">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1352,4 +1603,343 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3823986B-E9F6-4826-9D74-B16FD2828C7B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF065B6-A3EC-4C22-B232-59BB1EA66804}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16B6CC2-3C95-4FCE-892A-EDD1FDCD0CC5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB38131A-F41B-4F96-9D0E-EFE8A769AF32}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B6EA5A-9FC2-4084-A707-EDABA2BBDC06}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="66.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EB647E-4190-464B-8029-7FFD2C4C16EC}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C645274-1A31-4362-812E-1DD837CAEF37}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
playing with generated rule-based templates
</commit_message>
<xml_diff>
--- a/reports/corpus.xlsx
+++ b/reports/corpus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avitsas\Documents\thesis-backup\thesis\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AEFDA1-C3BB-4A68-A889-12AB60DA3953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2189005-2B09-42F9-BC73-F890AA4CA869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{187E2C83-AA30-4404-8C1D-88DFE9242203}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{187E2C83-AA30-4404-8C1D-88DFE9242203}"/>
   </bookViews>
   <sheets>
     <sheet name="corpus" sheetId="1" r:id="rId1"/>
@@ -2101,7 +2101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2319FDA2-137D-4D14-B1AA-140122FAA04B}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
@@ -3049,893 +3049,900 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E941BC9-72C2-4FF3-BFB6-CB4393649876}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="42.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>93</v>
       </c>
       <c r="B1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>93</v>
       </c>
-      <c r="D1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" vm="1">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s" vm="1">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>122</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s" vm="2">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" t="s" vm="85">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s" vm="3">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" t="s" vm="86">
+        <v>147</v>
+      </c>
+      <c r="D5" t="s" vm="4">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s" vm="87">
+        <v>148</v>
+      </c>
+      <c r="D6" t="s" vm="5">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" t="s" vm="88">
+        <v>149</v>
+      </c>
+      <c r="D7" t="s" vm="6">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s" vm="89">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s" vm="7">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s" vm="90">
+        <v>151</v>
+      </c>
+      <c r="D9" t="s" vm="8">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s" vm="91">
+        <v>152</v>
+      </c>
+      <c r="D10" t="s" vm="9">
+        <v>102</v>
+      </c>
+      <c r="E10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s" vm="92">
+        <v>121</v>
+      </c>
+      <c r="D11" t="s" vm="10">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" vm="2">
+      <c r="C12" s="1"/>
+      <c r="D12" t="s" vm="11">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s" vm="93">
+        <v>146</v>
+      </c>
+      <c r="D13" t="s" vm="12">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" t="s" vm="94">
+        <v>147</v>
+      </c>
+      <c r="D14" t="s" vm="13">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s" vm="95">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s" vm="14">
+        <v>107</v>
+      </c>
+      <c r="E15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s" vm="96">
+        <v>149</v>
+      </c>
+      <c r="D16" t="s" vm="15">
+        <v>108</v>
+      </c>
+      <c r="E16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s" vm="97">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s" vm="16">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s" vm="98">
+        <v>151</v>
+      </c>
+      <c r="D18" t="s" vm="17">
+        <v>110</v>
+      </c>
+      <c r="E18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s" vm="99">
+        <v>152</v>
+      </c>
+      <c r="D19" t="s" vm="18">
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s" vm="100">
+        <v>121</v>
+      </c>
+      <c r="D20" t="s" vm="19">
+        <v>112</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" t="s" vm="20">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s" vm="101">
+        <v>146</v>
+      </c>
+      <c r="D22" t="s" vm="21">
+        <v>114</v>
+      </c>
+      <c r="E22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="s" vm="102">
+        <v>147</v>
+      </c>
+      <c r="D23" t="s" vm="22">
+        <v>115</v>
+      </c>
+      <c r="E23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s" vm="103">
+        <v>148</v>
+      </c>
+      <c r="D24" t="s" vm="23">
+        <v>116</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s" vm="104">
+        <v>149</v>
+      </c>
+      <c r="D25" t="s" vm="24">
+        <v>117</v>
+      </c>
+      <c r="E25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s" vm="105">
+        <v>150</v>
+      </c>
+      <c r="D26" t="s" vm="25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s" vm="106">
+        <v>151</v>
+      </c>
+      <c r="D27" t="s" vm="26">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s" vm="107">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s" vm="27">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s" vm="108">
+        <v>121</v>
+      </c>
+      <c r="D29" t="s" vm="28">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" t="s" vm="109">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s" vm="29">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" t="s" vm="110">
+        <v>147</v>
+      </c>
+      <c r="D32" t="s" vm="30">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s" vm="111">
+        <v>148</v>
+      </c>
+      <c r="D33" t="s" vm="31">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s" vm="112">
+        <v>149</v>
+      </c>
+      <c r="D34" t="s" vm="32">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s" vm="113">
+        <v>150</v>
+      </c>
+      <c r="D35" t="s" vm="33">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s" vm="114">
+        <v>151</v>
+      </c>
+      <c r="D36" t="s" vm="34">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s" vm="115">
+        <v>152</v>
+      </c>
+      <c r="D37" t="s" vm="35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s" vm="116">
+        <v>121</v>
+      </c>
+      <c r="D38" t="s" vm="36">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" t="s" vm="37">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s" vm="109">
+        <v>146</v>
+      </c>
+      <c r="D40" t="s" vm="38">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s" vm="110">
+        <v>147</v>
+      </c>
+      <c r="D41" t="s" vm="39">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s" vm="111">
+        <v>148</v>
+      </c>
+      <c r="D42" t="s" vm="40">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s" vm="112">
+        <v>149</v>
+      </c>
+      <c r="D43" t="s" vm="41">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s" vm="113">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s" vm="42">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s" vm="114">
+        <v>151</v>
+      </c>
+      <c r="D45" t="s" vm="43">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s" vm="115">
+        <v>152</v>
+      </c>
+      <c r="D46" t="s" vm="44">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s" vm="116">
+        <v>121</v>
+      </c>
+      <c r="D47" t="s" vm="45">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s" vm="117">
+        <v>121</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" t="s" vm="46">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" t="s" vm="118">
+        <v>121</v>
+      </c>
+      <c r="D49" t="s" vm="47">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" t="s" vm="119">
+        <v>146</v>
+      </c>
+      <c r="D50" t="s" vm="48">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" t="s" vm="120">
+        <v>147</v>
+      </c>
+      <c r="D51" t="s" vm="49">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B52" t="s" vm="121">
+        <v>148</v>
+      </c>
+      <c r="D52" t="s" vm="50">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" t="s" vm="122">
+        <v>149</v>
+      </c>
+      <c r="D53" t="s" vm="51">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s" vm="123">
+        <v>150</v>
+      </c>
+      <c r="D54" t="s" vm="52">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B55" t="s" vm="124">
+        <v>151</v>
+      </c>
+      <c r="D55" t="s" vm="53">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B56" t="s" vm="125">
+        <v>152</v>
+      </c>
+      <c r="D56" t="s" vm="54">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" t="s" vm="126">
+        <v>121</v>
+      </c>
+      <c r="D57" t="s" vm="55">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" t="s" vm="127">
+        <v>144</v>
+      </c>
+      <c r="D58" t="s" vm="56">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" vm="3">
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D60" t="s" vm="57">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D61" t="s" vm="58">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D62" t="s" vm="59">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" t="s" vm="85">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" vm="4">
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s" vm="60">
         <v>97</v>
       </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" t="s" vm="86">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" vm="5">
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D64" t="s" vm="61">
         <v>98</v>
       </c>
-      <c r="B6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" t="s" vm="87">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" vm="6">
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" t="s" vm="62">
         <v>99</v>
       </c>
-      <c r="B7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" t="s" vm="88">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" vm="7">
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" t="s" vm="63">
         <v>100</v>
       </c>
-      <c r="B8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" t="s" vm="89">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" vm="8">
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" t="s" vm="64">
         <v>101</v>
       </c>
-      <c r="B9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" t="s" vm="90">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" vm="9">
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" t="s" vm="65">
         <v>102</v>
       </c>
-      <c r="B10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" t="s" vm="91">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" vm="10">
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" t="s" vm="66">
         <v>103</v>
       </c>
-      <c r="B11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" t="s" vm="92">
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" t="s" vm="67">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" t="s" vm="68">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" t="s" vm="69">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D73" t="s" vm="70">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D74" t="s" vm="71">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D75" t="s" vm="72">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D76" t="s" vm="73">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D77" t="s" vm="74">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D78" t="s" vm="75">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D79" t="s" vm="76">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D80" t="s" vm="77">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D81" t="s" vm="78">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D82" t="s" vm="79">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D83" t="s" vm="80">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D84" t="s" vm="81">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D85" t="s" vm="82">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D86" t="s" vm="83">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D87" t="s" vm="84">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" vm="11">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D88" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D89" t="s" vm="57">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D90" t="s" vm="58">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D91" t="s" vm="59">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D92" t="s" vm="60">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D93" t="s" vm="61">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D94" t="s" vm="62">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D95" t="s" vm="63">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D96" t="s" vm="64">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" t="s" vm="65">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" t="s" vm="66">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" t="s" vm="67">
         <v>104</v>
       </c>
-      <c r="B12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" vm="12">
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" t="s" vm="68">
         <v>105</v>
       </c>
-      <c r="B13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" t="s" vm="93">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" vm="13">
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" t="s" vm="69">
         <v>106</v>
       </c>
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" t="s" vm="94">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" vm="14">
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" t="s" vm="70">
         <v>107</v>
       </c>
-      <c r="B15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" t="s" vm="95">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" vm="15">
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" t="s" vm="71">
         <v>108</v>
       </c>
-      <c r="B16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" t="s" vm="96">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" vm="16">
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" t="s" vm="72">
         <v>109</v>
       </c>
-      <c r="B17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" t="s" vm="97">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" vm="17">
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" t="s" vm="73">
         <v>110</v>
       </c>
-      <c r="B18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" t="s" vm="98">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s" vm="18">
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" t="s" vm="74">
         <v>111</v>
       </c>
-      <c r="B19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D19" t="s" vm="99">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s" vm="19">
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D107" t="s" vm="75">
         <v>112</v>
       </c>
-      <c r="B20" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" t="s" vm="100">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s" vm="20">
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D108" t="s" vm="76">
         <v>113</v>
       </c>
-      <c r="B21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s" vm="21">
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D109" t="s" vm="77">
         <v>114</v>
       </c>
-      <c r="B22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" t="s" vm="101">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s" vm="22">
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D110" t="s" vm="78">
         <v>115</v>
       </c>
-      <c r="B23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D23" t="s" vm="102">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s" vm="23">
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D111" t="s" vm="79">
         <v>116</v>
       </c>
-      <c r="B24" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" t="s" vm="103">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s" vm="24">
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D112" t="s" vm="80">
         <v>117</v>
       </c>
-      <c r="B25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" t="s" vm="104">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s" vm="25">
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D113" t="s" vm="81">
         <v>118</v>
       </c>
-      <c r="D26" t="s" vm="105">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s" vm="26">
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D114" t="s" vm="82">
         <v>119</v>
       </c>
-      <c r="D27" t="s" vm="106">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s" vm="27">
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D115" t="s" vm="83">
         <v>120</v>
       </c>
-      <c r="D28" t="s" vm="107">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s" vm="28">
-        <v>121</v>
-      </c>
-      <c r="D29" t="s" vm="108">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s" vm="29">
-        <v>94</v>
-      </c>
-      <c r="D31" t="s" vm="109">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s" vm="30">
-        <v>95</v>
-      </c>
-      <c r="D32" t="s" vm="110">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s" vm="31">
-        <v>96</v>
-      </c>
-      <c r="D33" t="s" vm="111">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s" vm="32">
-        <v>97</v>
-      </c>
-      <c r="D34" t="s" vm="112">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s" vm="33">
-        <v>98</v>
-      </c>
-      <c r="D35" t="s" vm="113">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s" vm="34">
-        <v>99</v>
-      </c>
-      <c r="D36" t="s" vm="114">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s" vm="35">
-        <v>100</v>
-      </c>
-      <c r="D37" t="s" vm="115">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s" vm="36">
-        <v>101</v>
-      </c>
-      <c r="D38" t="s" vm="116">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s" vm="37">
-        <v>102</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s" vm="38">
-        <v>103</v>
-      </c>
-      <c r="D40" t="s" vm="109">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s" vm="39">
-        <v>104</v>
-      </c>
-      <c r="D41" t="s" vm="110">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s" vm="40">
-        <v>105</v>
-      </c>
-      <c r="D42" t="s" vm="111">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s" vm="41">
-        <v>106</v>
-      </c>
-      <c r="D43" t="s" vm="112">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s" vm="42">
-        <v>107</v>
-      </c>
-      <c r="D44" t="s" vm="113">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s" vm="43">
-        <v>108</v>
-      </c>
-      <c r="D45" t="s" vm="114">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s" vm="44">
-        <v>109</v>
-      </c>
-      <c r="D46" t="s" vm="115">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s" vm="45">
-        <v>110</v>
-      </c>
-      <c r="D47" t="s" vm="116">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s" vm="46">
-        <v>111</v>
-      </c>
-      <c r="D48" s="1" t="s" vm="117">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s" vm="47">
-        <v>112</v>
-      </c>
-      <c r="D49" t="s" vm="118">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s" vm="48">
-        <v>113</v>
-      </c>
-      <c r="D50" t="s" vm="119">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s" vm="49">
-        <v>114</v>
-      </c>
-      <c r="D51" t="s" vm="120">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s" vm="50">
-        <v>115</v>
-      </c>
-      <c r="D52" t="s" vm="121">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s" vm="51">
-        <v>116</v>
-      </c>
-      <c r="D53" t="s" vm="122">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s" vm="52">
-        <v>117</v>
-      </c>
-      <c r="D54" t="s" vm="123">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s" vm="53">
-        <v>118</v>
-      </c>
-      <c r="D55" t="s" vm="124">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s" vm="54">
-        <v>119</v>
-      </c>
-      <c r="D56" t="s" vm="125">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s" vm="55">
-        <v>120</v>
-      </c>
-      <c r="D57" t="s" vm="126">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s" vm="56">
-        <v>121</v>
-      </c>
-      <c r="D58" t="s" vm="127">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s" vm="57">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s" vm="58">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s" vm="59">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s" vm="60">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s" vm="61">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s" vm="62">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s" vm="63">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s" vm="64">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s" vm="65">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s" vm="66">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s" vm="67">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s" vm="68">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s" vm="69">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s" vm="70">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s" vm="71">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s" vm="72">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s" vm="73">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s" vm="74">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s" vm="75">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s" vm="76">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s" vm="77">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s" vm="78">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s" vm="79">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s" vm="80">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s" vm="81">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s" vm="82">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s" vm="83">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s" vm="84">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s" vm="57">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s" vm="58">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s" vm="59">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s" vm="60">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s" vm="61">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s" vm="62">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s" vm="63">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s" vm="64">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s" vm="65">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s" vm="66">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s" vm="67">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s" vm="68">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s" vm="69">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s" vm="70">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s" vm="71">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s" vm="72">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s" vm="73">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s" vm="74">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s" vm="75">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s" vm="76">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s" vm="77">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s" vm="78">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" t="s" vm="79">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" t="s" vm="80">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s" vm="81">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" t="s" vm="82">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" t="s" vm="83">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" t="s" vm="84">
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D116" t="s" vm="84">
         <v>121</v>
       </c>
     </row>

</xml_diff>